<commit_message>
update bieu do 2
</commit_message>
<xml_diff>
--- a/public/baoCaoXNT/05_2024.xlsx
+++ b/public/baoCaoXNT/05_2024.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="16">
   <si>
     <t>Báo cáo xuất nhập tồn</t>
   </si>
@@ -29,6 +29,9 @@
     <t>Tên sản phẩm</t>
   </si>
   <si>
+    <t>Mã danh mục</t>
+  </si>
+  <si>
     <t>Tồn đầu kỳ</t>
   </si>
   <si>
@@ -57,6 +60,9 @@
   </si>
   <si>
     <t>Smart Tivi LG 4K 55 inch 55UQ8000PSC</t>
+  </si>
+  <si>
+    <t>may giat 1</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -410,9 +416,10 @@
     <col min="4" max="4" width="10" customWidth="true" style="0"/>
     <col min="5" max="5" width="10" customWidth="true" style="0"/>
     <col min="6" max="6" width="10" customWidth="true" style="0"/>
+    <col min="7" max="7" width="10" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -420,7 +427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -439,36 +446,42 @@
       <c r="F2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>25</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>6</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -479,16 +492,19 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -499,16 +515,19 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -519,16 +538,19 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -539,16 +561,19 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -557,13 +582,39 @@
         <v>0</v>
       </c>
       <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>34</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells>
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:F1"/>
+    <mergeCell ref="C1:G1"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bieu do sua 1
</commit_message>
<xml_diff>
--- a/public/baoCaoXNT/05_2024.xlsx
+++ b/public/baoCaoXNT/05_2024.xlsx
@@ -602,13 +602,13 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F9">
         <v>0</v>
       </c>
       <c r="G9">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>